<commit_message>
rerun with more pics
</commit_message>
<xml_diff>
--- a/results/FigureLabels.xlsx
+++ b/results/FigureLabels.xlsx
@@ -57,6 +57,9 @@
     <t>legends</t>
   </si>
   <si>
+    <t>to</t>
+  </si>
+  <si>
     <t>of</t>
   </si>
   <si>
@@ -66,13 +69,10 @@
     <t>officers</t>
   </si>
   <si>
-    <t>to</t>
+    <t>police</t>
   </si>
   <si>
     <t>in</t>
-  </si>
-  <si>
-    <t>police</t>
   </si>
   <si>
     <t>Mar</t>
@@ -187,7 +187,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="avgbar.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="avgbar1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -719,10 +719,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>